<commit_message>
added delete & update functions of CRUD
</commit_message>
<xml_diff>
--- a/New SQLite! Attributes' Types and Names.xlsx
+++ b/New SQLite! Attributes' Types and Names.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YBeesMacBookPro/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YBeesMacBookPro/Google Drive/CS 542/hotelmanager/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="460" windowWidth="14320" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="167">
   <si>
     <t>Table1</t>
   </si>
@@ -110,15 +110,9 @@
     <t>DOB</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>dob</t>
   </si>
   <si>
-    <t>DATE</t>
-  </si>
-  <si>
     <t>MM/DD/YYYY ONLY FOR THE MEMBERS</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>checkInDate</t>
   </si>
   <si>
-    <t>MM/DD/YYYY  *</t>
-  </si>
-  <si>
     <t>check-out Date</t>
   </si>
   <si>
@@ -518,19 +509,25 @@
     <t>6Num*</t>
   </si>
   <si>
-    <t>DateTime</t>
-  </si>
-  <si>
     <t>3Num</t>
   </si>
   <si>
-    <t>20Num*</t>
-  </si>
-  <si>
     <t>3Num*</t>
   </si>
   <si>
     <t>10Num*</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DDTHH:MM</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>F/M</t>
+  </si>
+  <si>
+    <t>8Num*</t>
   </si>
 </sst>
 </file>
@@ -542,7 +539,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -873,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,7 +880,7 @@
     <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" customWidth="1"/>
     <col min="5" max="5" width="23.83203125" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" customWidth="1"/>
+    <col min="8" max="8" width="65" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -989,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -997,13 +994,13 @@
         <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>8</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -1017,71 +1014,71 @@
         <v>26</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F8" s="5">
         <v>16</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1098,53 +1095,53 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
-        <v>145</v>
-      </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1153,109 +1150,109 @@
         <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F15">
         <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>50</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F16">
         <v>8</v>
       </c>
       <c r="H16" t="s">
-        <v>50</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1272,86 +1269,86 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" t="s">
         <v>42</v>
       </c>
-      <c r="C22" t="s">
-        <v>145</v>
-      </c>
-      <c r="D22" t="s">
-        <v>44</v>
-      </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G22" t="s">
         <v>11</v>
       </c>
       <c r="H22" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F24" s="5"/>
       <c r="H24" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F25" s="5"/>
       <c r="H25" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>10</v>
@@ -1360,18 +1357,18 @@
         <v>10</v>
       </c>
       <c r="H26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>10</v>
@@ -1380,15 +1377,15 @@
         <v>30</v>
       </c>
       <c r="H27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -1408,50 +1405,50 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H30" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G31" t="s">
         <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1460,25 +1457,25 @@
         <v>30</v>
       </c>
       <c r="H32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F33" s="5"/>
       <c r="H33" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1498,7 +1495,7 @@
         <v>30</v>
       </c>
       <c r="H34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1518,10 +1515,10 @@
         <v>300</v>
       </c>
       <c r="G35" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H35" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1529,19 +1526,19 @@
         <v>24</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D36" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H36" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1566,27 +1563,27 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
@@ -1603,13 +1600,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1621,58 +1618,58 @@
         <v>11</v>
       </c>
       <c r="H41" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G42" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H42" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G43" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H43" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -1681,36 +1678,36 @@
         <v>10</v>
       </c>
       <c r="H44" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D45" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F45" s="5"/>
       <c r="H45" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
@@ -1719,69 +1716,69 @@
         <v>10</v>
       </c>
       <c r="H46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D48" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E48" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H48" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="D49" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F49">
         <v>8</v>
       </c>
       <c r="H49" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -1798,13 +1795,13 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
@@ -1816,38 +1813,38 @@
         <v>11</v>
       </c>
       <c r="H52" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C53" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D53" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G53" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H53" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E54" t="s">
         <v>10</v>
@@ -1856,72 +1853,72 @@
         <v>10</v>
       </c>
       <c r="H54" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C55" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D55" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E55" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G55" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H55" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C56" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D56" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E56" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H56" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="D57" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E57" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F57">
         <v>8</v>
       </c>
       <c r="H57" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -1938,13 +1935,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B60" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>10</v>
@@ -1958,13 +1955,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C61" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>10</v>
@@ -1975,13 +1972,13 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C62" t="s">
         <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E62" t="s">
         <v>10</v>
@@ -1992,30 +1989,33 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C63" t="s">
+        <v>142</v>
+      </c>
+      <c r="D63" t="s">
+        <v>101</v>
+      </c>
+      <c r="E63" t="s">
+        <v>43</v>
+      </c>
+      <c r="F63">
+        <v>13</v>
+      </c>
+      <c r="H63" t="s">
         <v>163</v>
-      </c>
-      <c r="D63" t="s">
-        <v>104</v>
-      </c>
-      <c r="E63" t="s">
-        <v>163</v>
-      </c>
-      <c r="F63">
-        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E64" t="s">
         <v>10</v>
@@ -2026,16 +2026,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D65" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E65" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F65">
         <v>3</v>
@@ -2043,27 +2043,27 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D66" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E66" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C67" t="s">
         <v>8</v>
       </c>
       <c r="D67" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E67" t="s">
         <v>10</v>
@@ -2074,10 +2074,10 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C69" t="s">
         <v>2</v>
@@ -2094,13 +2094,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B70" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C70" t="s">
         <v>8</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>10</v>
@@ -2114,13 +2114,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
       </c>
       <c r="D71" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E71" t="s">
         <v>10</v>
@@ -2131,13 +2131,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C72" t="s">
         <v>8</v>
       </c>
       <c r="D72" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E72" t="s">
         <v>10</v>
@@ -2148,47 +2148,47 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C73" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D73" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E73" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H73" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C74" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D74" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E74" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C75" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="D75" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E75" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F75">
         <v>8</v>
@@ -2196,16 +2196,16 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C76" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D76" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E76" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F76">
         <v>8</v>
@@ -2213,13 +2213,13 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C77" t="s">
         <v>8</v>
       </c>
       <c r="D77" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E77" t="s">
         <v>10</v>
@@ -2230,13 +2230,13 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
       </c>
       <c r="D78" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E78" t="s">
         <v>10</v>
@@ -2247,13 +2247,13 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E79" t="s">
         <v>10</v>
@@ -2264,10 +2264,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C81" t="s">
         <v>2</v>
@@ -2284,22 +2284,22 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B82" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C82" t="s">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="D82" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E82" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G82" t="s">
         <v>11</v>
       </c>
       <c r="H82" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2321,30 +2321,30 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C84" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D84" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E84" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H84" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
       </c>
       <c r="D85" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E85" t="s">
         <v>10</v>
@@ -2355,16 +2355,16 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C86" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="D86" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E86" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F86">
         <v>8</v>
@@ -2372,16 +2372,16 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C87" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="D87" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E87" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F87">
         <v>8</v>
@@ -2389,10 +2389,10 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C89" t="s">
         <v>2</v>
@@ -2409,13 +2409,13 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C90" t="s">
         <v>8</v>
       </c>
       <c r="D90" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E90" t="s">
         <v>10</v>
@@ -2426,13 +2426,13 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C91" t="s">
         <v>8</v>
       </c>
       <c r="D91" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E91" t="s">
         <v>10</v>
@@ -2443,33 +2443,33 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C92" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D92" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E92" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H92" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C93" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="D93" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E93" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F93">
         <v>8</v>
@@ -2477,16 +2477,16 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C94" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="D94" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E94" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F94">
         <v>8</v>
@@ -2494,22 +2494,22 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B95" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C95" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D95" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E95" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G95" t="s">
         <v>11</v>
       </c>
       <c r="H95" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
mock data added to database
</commit_message>
<xml_diff>
--- a/New SQLite! Attributes' Types and Names.xlsx
+++ b/New SQLite! Attributes' Types and Names.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="166">
   <si>
     <t>Table1</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>BOOLEAN</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>reusable</t>
   </si>
   <si>
-    <t>Y/N *</t>
-  </si>
-  <si>
     <t>cost</t>
   </si>
   <si>
@@ -525,6 +519,12 @@
   </si>
   <si>
     <t>SCHED</t>
+  </si>
+  <si>
+    <t>customer_ssn</t>
+  </si>
+  <si>
+    <t>0/1</t>
   </si>
 </sst>
 </file>
@@ -867,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,7 +974,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
@@ -983,99 +983,99 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" s="5">
         <v>16</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1092,53 +1092,53 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
-      </c>
       <c r="E12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" t="s">
         <v>138</v>
       </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
         <v>42</v>
-      </c>
-      <c r="G13" t="s">
-        <v>139</v>
-      </c>
-      <c r="H13" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>43</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1147,109 +1147,109 @@
         <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
-      </c>
       <c r="E15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15">
         <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
-      </c>
       <c r="E16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16">
         <v>8</v>
       </c>
       <c r="H16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H17" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>141</v>
-      </c>
-      <c r="H17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D19" t="s">
-        <v>53</v>
-      </c>
       <c r="E19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1266,106 +1266,106 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G22" t="s">
         <v>11</v>
       </c>
       <c r="H22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" t="s">
-        <v>141</v>
-      </c>
-      <c r="D23" t="s">
-        <v>58</v>
-      </c>
       <c r="E23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" s="5"/>
       <c r="H24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" t="s">
         <v>60</v>
       </c>
-      <c r="C25" t="s">
-        <v>138</v>
-      </c>
-      <c r="D25" t="s">
-        <v>61</v>
-      </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F25" s="5"/>
       <c r="H25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="H26" t="s">
         <v>62</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26">
-        <v>10</v>
-      </c>
-      <c r="H26" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>10</v>
@@ -1374,15 +1374,15 @@
         <v>30</v>
       </c>
       <c r="H27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -1402,50 +1402,50 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C31" t="s">
-        <v>138</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="E31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G31" t="s">
         <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1454,25 +1454,25 @@
         <v>30</v>
       </c>
       <c r="H32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" t="s">
         <v>70</v>
       </c>
-      <c r="C33" t="s">
-        <v>138</v>
-      </c>
-      <c r="D33" t="s">
-        <v>71</v>
-      </c>
       <c r="E33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F33" s="5"/>
       <c r="H33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1492,7 +1492,7 @@
         <v>30</v>
       </c>
       <c r="H34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1512,30 +1512,30 @@
         <v>300</v>
       </c>
       <c r="G35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1546,7 +1546,7 @@
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1555,32 +1555,32 @@
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
@@ -1597,13 +1597,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1615,97 +1615,97 @@
         <v>11</v>
       </c>
       <c r="H41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" t="s">
         <v>67</v>
       </c>
-      <c r="C42" t="s">
-        <v>138</v>
-      </c>
-      <c r="D42" t="s">
-        <v>68</v>
-      </c>
       <c r="E42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G43" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H43" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44">
+        <v>10</v>
+      </c>
+      <c r="H44" t="s">
         <v>77</v>
-      </c>
-      <c r="C44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44">
-        <v>10</v>
-      </c>
-      <c r="H44" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" t="s">
         <v>79</v>
       </c>
-      <c r="C45" t="s">
-        <v>138</v>
-      </c>
-      <c r="D45" t="s">
-        <v>80</v>
-      </c>
       <c r="E45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F45" s="5"/>
       <c r="H45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
         <v>81</v>
       </c>
-      <c r="C46" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" t="s">
-        <v>82</v>
-      </c>
       <c r="E46" t="s">
         <v>10</v>
       </c>
@@ -1713,69 +1713,69 @@
         <v>10</v>
       </c>
       <c r="H46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="D47" t="s">
-        <v>83</v>
-      </c>
-      <c r="F47">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="E47" t="s">
+        <v>41</v>
       </c>
       <c r="H47" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D48" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E48" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H48" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D49" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F49">
         <v>8</v>
       </c>
       <c r="H49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -1792,13 +1792,13 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
@@ -1810,38 +1810,38 @@
         <v>11</v>
       </c>
       <c r="H52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D53" t="s">
         <v>67</v>
       </c>
-      <c r="C53" t="s">
-        <v>138</v>
-      </c>
-      <c r="D53" t="s">
-        <v>68</v>
-      </c>
       <c r="E53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G53" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H53" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E54" t="s">
         <v>10</v>
@@ -1850,72 +1850,72 @@
         <v>10</v>
       </c>
       <c r="H54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D55" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G55" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H55" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C56" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D56" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E56" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D57" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F57">
         <v>8</v>
       </c>
       <c r="H57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -1932,13 +1932,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B60" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>10</v>
@@ -1949,13 +1949,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C61" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>10</v>
@@ -1969,13 +1969,13 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C62" t="s">
         <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E62" t="s">
         <v>10</v>
@@ -1986,33 +1986,33 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C63" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D63" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F63">
         <v>13</v>
       </c>
       <c r="H63" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E64" t="s">
         <v>10</v>
@@ -2023,16 +2023,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C65" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F65">
         <v>3</v>
@@ -2040,27 +2040,27 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C66" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D66" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E66" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C67" t="s">
         <v>8</v>
       </c>
       <c r="D67" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E67" t="s">
         <v>10</v>
@@ -2071,10 +2071,10 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C69" t="s">
         <v>2</v>
@@ -2091,13 +2091,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B70" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C70" t="s">
         <v>8</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E70" t="s">
         <v>10</v>
@@ -2111,13 +2111,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B71" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>10</v>
@@ -2128,13 +2128,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C72" t="s">
         <v>8</v>
       </c>
       <c r="D72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E72" t="s">
         <v>10</v>
@@ -2145,13 +2145,13 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C73" t="s">
         <v>8</v>
       </c>
       <c r="D73" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E73" t="s">
         <v>10</v>
@@ -2162,47 +2162,47 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C74" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E74" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H74" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C75" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D75" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E75" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C76" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D76" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E76" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F76">
         <v>8</v>
@@ -2210,16 +2210,16 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C77" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D77" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E77" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F77">
         <v>8</v>
@@ -2227,13 +2227,13 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
       </c>
       <c r="D78" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E78" t="s">
         <v>10</v>
@@ -2244,13 +2244,13 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E79" t="s">
         <v>10</v>
@@ -2261,13 +2261,13 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C80" t="s">
         <v>8</v>
       </c>
       <c r="D80" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E80" t="s">
         <v>10</v>
@@ -2278,10 +2278,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C82" t="s">
         <v>2</v>
@@ -2298,22 +2298,22 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B83" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C83" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D83" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E83" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G83" t="s">
         <v>11</v>
       </c>
       <c r="H83" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -2335,30 +2335,30 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C85" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D85" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E85" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H85" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C86" t="s">
         <v>8</v>
       </c>
       <c r="D86" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E86" t="s">
         <v>10</v>
@@ -2369,16 +2369,16 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C87" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D87" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E87" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F87">
         <v>8</v>
@@ -2386,16 +2386,16 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C88" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D88" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E88" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F88">
         <v>8</v>
@@ -2403,10 +2403,10 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C90" t="s">
         <v>2</v>
@@ -2423,13 +2423,13 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C91" t="s">
         <v>8</v>
       </c>
       <c r="D91" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E91" t="s">
         <v>10</v>
@@ -2440,13 +2440,13 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
       </c>
       <c r="D92" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E92" t="s">
         <v>10</v>
@@ -2457,33 +2457,33 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C93" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D93" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E93" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H93" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C94" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D94" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E94" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F94">
         <v>8</v>
@@ -2491,16 +2491,16 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C95" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D95" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E95" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F95">
         <v>8</v>
@@ -2508,22 +2508,22 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B96" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C96" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D96" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E96" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G96" t="s">
         <v>11</v>
       </c>
       <c r="H96" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
altered templates to fix the new database
</commit_message>
<xml_diff>
--- a/New SQLite! Attributes' Types and Names.xlsx
+++ b/New SQLite! Attributes' Types and Names.xlsx
@@ -531,7 +531,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -562,6 +562,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -583,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -593,6 +601,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1931,7 +1940,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="6" t="s">
         <v>92</v>
       </c>
       <c r="C60" t="s">
@@ -1948,7 +1957,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+      <c r="B61" s="7" t="s">
         <v>163</v>
       </c>
       <c r="C61" t="s">
@@ -2090,7 +2099,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C70" t="s">
@@ -2110,7 +2119,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="6" t="s">
         <v>92</v>
       </c>
       <c r="C71" t="s">

</xml_diff>